<commit_message>
- change to SI units
</commit_message>
<xml_diff>
--- a/Lucie_Ductility_Data.xlsx
+++ b/Lucie_Ductility_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="146">
   <si>
     <t>Metadata</t>
   </si>
@@ -293,99 +293,57 @@
     <t>compressive ductility</t>
   </si>
   <si>
-    <t>2.10E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.intermet.2011.01.004</t>
   </si>
   <si>
     <t>V Nb Ta Mo W</t>
   </si>
   <si>
-    <t>1.70E-02</t>
-  </si>
-  <si>
-    <t>8.80E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.msea.2017.12.021</t>
   </si>
   <si>
     <t>Ti Zr Hf Nb Mo</t>
   </si>
   <si>
-    <t>1.01E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.intermet.2015.10.011</t>
   </si>
   <si>
     <t>Ti Zr Hf Nb0.5 Mo</t>
   </si>
   <si>
-    <t>1.30E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf Nb1.5 Mo</t>
   </si>
   <si>
-    <t>2.40E-01</t>
-  </si>
-  <si>
     <t>Ti0.5  Zr Hf Nb Mo</t>
   </si>
   <si>
-    <t>1.21E-01</t>
-  </si>
-  <si>
     <t>Ti1.5 Zr Hf Nb Mo</t>
   </si>
   <si>
-    <t>2.90E-01</t>
-  </si>
-  <si>
     <t>Ti Zr0.5 Hf Nb Mo</t>
   </si>
   <si>
-    <t>1.80E-01</t>
-  </si>
-  <si>
     <t>Ti Zr1.5 Hf Nb Mo</t>
   </si>
   <si>
-    <t>1.61E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf0.5 Nb Mo</t>
   </si>
   <si>
     <t>Ti Zr Hf1.5 Nb Mo</t>
   </si>
   <si>
-    <t>1.68E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf0.5 Nb Mo0.5</t>
   </si>
   <si>
-    <t>2.46E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf Nb Mo1.5</t>
   </si>
   <si>
-    <t>1.08E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf Nb Ta</t>
   </si>
   <si>
     <t>at least</t>
   </si>
   <si>
-    <t>5.00E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.jallcom.2011.02.171</t>
   </si>
   <si>
@@ -410,51 +368,30 @@
     <t>Ti Zr Hf Nb Ta Mo</t>
   </si>
   <si>
-    <t>1.20E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Nb Mo</t>
   </si>
   <si>
-    <t>3.30E-01</t>
-  </si>
-  <si>
     <t>10.1007/s11837-012-0366-5</t>
   </si>
   <si>
     <t>Ti Zr V0.25 Nb Mo</t>
   </si>
   <si>
-    <t>3.00E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V0.5 Nb Mo</t>
   </si>
   <si>
-    <t>2.80E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V0.75 Nb Mo</t>
   </si>
   <si>
     <t>Ti Zr V Nb Mo</t>
   </si>
   <si>
-    <t>2.60E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V1.5 Nb Mo</t>
   </si>
   <si>
-    <t>2.00E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V2 Nb Mo</t>
   </si>
   <si>
-    <t>2.30E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V3 Nb Mo</t>
   </si>
   <si>
@@ -482,63 +419,36 @@
     <t>Ti V Nb Mo</t>
   </si>
   <si>
-    <t>2.56E-01</t>
-  </si>
-  <si>
     <t>Ti Zr Hf V Nb</t>
   </si>
   <si>
-    <t>2.96E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.ijrmhm.2014.07.009</t>
   </si>
   <si>
-    <t>1.02E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.matdes.2015.05.019</t>
   </si>
   <si>
     <t>Ti V Nb Ta Mo W</t>
   </si>
   <si>
-    <t>1.06E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.intermet.2017.01.007</t>
   </si>
   <si>
     <t>Ti Nb Ta Mo W</t>
   </si>
   <si>
-    <t>1.41E-01</t>
-  </si>
-  <si>
-    <t>2.60E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.matdes.2015.06.072</t>
   </si>
   <si>
     <t>Ti Zr V0.3 Nb</t>
   </si>
   <si>
-    <t>4.50E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V Nb Mo0.3</t>
   </si>
   <si>
-    <t>4.20E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V Nb Mo0.5</t>
   </si>
   <si>
-    <t>3.20E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V Nb Mo0.7</t>
   </si>
   <si>
@@ -554,69 +464,39 @@
     <t>Ti Zr V0.3 Nb Mo0.5</t>
   </si>
   <si>
-    <t>4.30E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V0.3 Nb Mo0.7</t>
   </si>
   <si>
-    <t>2.66E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V0.3 Nb Mo1.0</t>
   </si>
   <si>
-    <t>2.50E-01</t>
-  </si>
-  <si>
     <t>Ti Zr V0.3 Nb Mo1.3</t>
   </si>
   <si>
     <t>Ti Zr V0.3 Nb Mo1.5</t>
   </si>
   <si>
-    <t>8.00E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.intermet.2015.09.011</t>
   </si>
   <si>
     <t>Zr Hf Nb Ta</t>
   </si>
   <si>
-    <t>3.40E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.actamat.2016.01.018</t>
   </si>
   <si>
-    <t>1.90E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.msea.2017.12.004</t>
   </si>
   <si>
     <t>Ti0.25 Nb Ta Mo W</t>
   </si>
   <si>
-    <t>2.50E-02</t>
-  </si>
-  <si>
     <t>Ti0.5 Nb Ta Mo W</t>
   </si>
   <si>
-    <t>5.90E-02</t>
-  </si>
-  <si>
     <t>Ti0.75 Nb Ta Mo W</t>
   </si>
   <si>
-    <t>8.40E-02</t>
-  </si>
-  <si>
-    <t>1.15E-01</t>
-  </si>
-  <si>
     <t>Ti V Nb Ta Mo</t>
   </si>
   <si>
@@ -629,31 +509,19 @@
     <t>tensile ductility</t>
   </si>
   <si>
-    <t>2.06E-01</t>
-  </si>
-  <si>
     <t>10.1038/s41563-020-0750-4</t>
   </si>
   <si>
-    <t>9.70E-02</t>
-  </si>
-  <si>
     <t>10.1016/j.jallcom.2015.07.209</t>
   </si>
   <si>
     <t>Ti Zr Hf Nb</t>
   </si>
   <si>
-    <t>1.49E-01</t>
-  </si>
-  <si>
     <t>10.1016/j.matlet.2014.09.044</t>
   </si>
   <si>
     <t>Ti1.5 ZrHf0.5 Nb0.5 Ta0.5</t>
-  </si>
-  <si>
-    <t>1.88E-01</t>
   </si>
   <si>
     <t>10.1063/1.4966659</t>
@@ -666,7 +534,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,12 +552,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1241,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1261,19 +1123,19 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1294,13 +1156,13 @@
     <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1321,64 +1183,64 @@
     <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
@@ -1423,52 +1285,52 @@
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="28" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="29" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="29" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="29" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="29" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="5" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="30" applyBorder="1" fontId="5" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="30" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="5" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="4" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1480,16 +1342,13 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1511,7 +1370,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,26 +1680,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="84" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="84" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="85" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="85" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="84" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="85" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="85" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="85" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="86" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="87" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="88" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="89" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="89" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="89" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="84" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="90" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="84" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="84" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="84" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="84" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="83" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="83" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="84" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="84" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="83" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="84" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="84" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="84" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="85" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="86" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="87" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="88" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="88" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="88" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="83" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="89" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="83" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="83" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="83" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="83" width="17.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.75">
@@ -2195,17 +2054,17 @@
       <c r="I10" s="78">
         <v>298</v>
       </c>
-      <c r="J10" s="79" t="s">
-        <v>68</v>
+      <c r="J10" s="79">
+        <v>2.1</v>
       </c>
       <c r="K10" s="79"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O10" s="5"/>
-      <c r="P10" s="80">
+      <c r="P10" s="7">
         <v>2.1</v>
       </c>
       <c r="Q10" s="2"/>
@@ -2216,7 +2075,7 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="77"/>
       <c r="B11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>66</v>
@@ -2233,17 +2092,17 @@
       <c r="I11" s="78">
         <v>298</v>
       </c>
-      <c r="J11" s="79" t="s">
-        <v>71</v>
+      <c r="J11" s="79">
+        <v>1.7</v>
       </c>
       <c r="K11" s="79"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O11" s="5"/>
-      <c r="P11" s="80">
+      <c r="P11" s="7">
         <v>1.7</v>
       </c>
       <c r="Q11" s="2"/>
@@ -2254,7 +2113,7 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="77"/>
       <c r="B12" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>66</v>
@@ -2271,17 +2130,17 @@
       <c r="I12" s="78">
         <v>298</v>
       </c>
-      <c r="J12" s="79" t="s">
-        <v>72</v>
+      <c r="J12" s="79">
+        <v>8.8</v>
       </c>
       <c r="K12" s="79"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="81" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" s="82"/>
-      <c r="P12" s="80">
+      <c r="N12" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="81"/>
+      <c r="P12" s="7">
         <v>8.8</v>
       </c>
       <c r="Q12" s="2"/>
@@ -2292,7 +2151,7 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="77"/>
       <c r="B13" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>66</v>
@@ -2309,17 +2168,17 @@
       <c r="I13" s="78">
         <v>298</v>
       </c>
-      <c r="J13" s="79" t="s">
-        <v>75</v>
+      <c r="J13" s="79">
+        <v>10.12</v>
       </c>
       <c r="K13" s="79"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="80">
+      <c r="P13" s="7">
         <v>10.12</v>
       </c>
       <c r="Q13" s="2"/>
@@ -2330,7 +2189,7 @@
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="77"/>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>66</v>
@@ -2347,17 +2206,17 @@
       <c r="I14" s="78">
         <v>298</v>
       </c>
-      <c r="J14" s="79" t="s">
-        <v>78</v>
+      <c r="J14" s="79">
+        <v>13.02</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O14" s="5"/>
-      <c r="P14" s="80">
+      <c r="P14" s="7">
         <v>13.02</v>
       </c>
       <c r="Q14" s="2"/>
@@ -2368,7 +2227,7 @@
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="77"/>
       <c r="B15" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>66</v>
@@ -2385,17 +2244,17 @@
       <c r="I15" s="78">
         <v>298</v>
       </c>
-      <c r="J15" s="79" t="s">
-        <v>80</v>
+      <c r="J15" s="79">
+        <v>23.97</v>
       </c>
       <c r="K15" s="79"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O15" s="5"/>
-      <c r="P15" s="80">
+      <c r="P15" s="7">
         <v>23.97</v>
       </c>
       <c r="Q15" s="2"/>
@@ -2406,7 +2265,7 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="77"/>
       <c r="B16" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
@@ -2423,17 +2282,17 @@
       <c r="I16" s="78">
         <v>298</v>
       </c>
-      <c r="J16" s="79" t="s">
-        <v>82</v>
+      <c r="J16" s="79">
+        <v>12.08</v>
       </c>
       <c r="K16" s="79"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O16" s="5"/>
-      <c r="P16" s="80">
+      <c r="P16" s="7">
         <v>12.08</v>
       </c>
       <c r="Q16" s="2"/>
@@ -2444,7 +2303,7 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="77"/>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>66</v>
@@ -2461,17 +2320,17 @@
       <c r="I17" s="78">
         <v>298</v>
       </c>
-      <c r="J17" s="79" t="s">
-        <v>84</v>
+      <c r="J17" s="79">
+        <v>28.98</v>
       </c>
       <c r="K17" s="79"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O17" s="2"/>
-      <c r="P17" s="80">
+      <c r="P17" s="7">
         <v>28.98</v>
       </c>
       <c r="Q17" s="2"/>
@@ -2482,7 +2341,7 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="77"/>
       <c r="B18" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>66</v>
@@ -2499,17 +2358,17 @@
       <c r="I18" s="78">
         <v>298</v>
       </c>
-      <c r="J18" s="79" t="s">
-        <v>86</v>
+      <c r="J18" s="79">
+        <v>18.02</v>
       </c>
       <c r="K18" s="79"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="80">
+      <c r="P18" s="7">
         <v>18.02</v>
       </c>
       <c r="Q18" s="2"/>
@@ -2520,7 +2379,7 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="77"/>
       <c r="B19" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>66</v>
@@ -2537,17 +2396,17 @@
       <c r="I19" s="78">
         <v>298</v>
       </c>
-      <c r="J19" s="79" t="s">
-        <v>88</v>
+      <c r="J19" s="79">
+        <v>16.09</v>
       </c>
       <c r="K19" s="79"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O19" s="2"/>
-      <c r="P19" s="80">
+      <c r="P19" s="7">
         <v>16.09</v>
       </c>
       <c r="Q19" s="2"/>
@@ -2558,7 +2417,7 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="77"/>
       <c r="B20" s="6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>66</v>
@@ -2575,17 +2434,17 @@
       <c r="I20" s="78">
         <v>298</v>
       </c>
-      <c r="J20" s="79" t="s">
-        <v>82</v>
+      <c r="J20" s="79">
+        <v>12.09</v>
       </c>
       <c r="K20" s="79"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="80">
+      <c r="P20" s="7">
         <v>12.09</v>
       </c>
       <c r="Q20" s="2"/>
@@ -2596,7 +2455,7 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="77"/>
       <c r="B21" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>66</v>
@@ -2613,17 +2472,17 @@
       <c r="I21" s="78">
         <v>298</v>
       </c>
-      <c r="J21" s="79" t="s">
-        <v>91</v>
+      <c r="J21" s="79">
+        <v>16.83</v>
       </c>
       <c r="K21" s="79"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O21" s="2"/>
-      <c r="P21" s="80">
+      <c r="P21" s="7">
         <v>16.83</v>
       </c>
       <c r="Q21" s="2"/>
@@ -2634,7 +2493,7 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="77"/>
       <c r="B22" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>66</v>
@@ -2651,17 +2510,17 @@
       <c r="I22" s="78">
         <v>298</v>
       </c>
-      <c r="J22" s="79" t="s">
-        <v>93</v>
+      <c r="J22" s="79">
+        <v>24.61</v>
       </c>
       <c r="K22" s="79"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O22" s="2"/>
-      <c r="P22" s="80">
+      <c r="P22" s="7">
         <v>24.61</v>
       </c>
       <c r="Q22" s="2"/>
@@ -2672,7 +2531,7 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="77"/>
       <c r="B23" s="6" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>66</v>
@@ -2689,17 +2548,17 @@
       <c r="I23" s="78">
         <v>298</v>
       </c>
-      <c r="J23" s="79" t="s">
-        <v>95</v>
+      <c r="J23" s="79">
+        <v>10.83</v>
       </c>
       <c r="K23" s="79"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="80">
+      <c r="P23" s="7">
         <v>10.83</v>
       </c>
       <c r="Q23" s="2"/>
@@ -2710,7 +2569,7 @@
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="77"/>
       <c r="B24" s="6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>66</v>
@@ -2724,23 +2583,23 @@
         <v>31</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I24" s="78">
         <v>298</v>
       </c>
-      <c r="J24" s="79" t="s">
-        <v>98</v>
+      <c r="J24" s="79">
+        <v>50</v>
       </c>
       <c r="K24" s="79"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="O24" s="2"/>
-      <c r="P24" s="83" t="s">
-        <v>100</v>
+      <c r="P24" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -2750,7 +2609,7 @@
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="77"/>
       <c r="B25" s="6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>66</v>
@@ -2764,23 +2623,23 @@
         <v>31</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I25" s="78">
         <v>298</v>
       </c>
-      <c r="J25" s="79" t="s">
-        <v>98</v>
+      <c r="J25" s="79">
+        <v>50</v>
       </c>
       <c r="K25" s="79"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O25" s="2"/>
-      <c r="P25" s="83" t="s">
-        <v>100</v>
+      <c r="P25" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -2790,7 +2649,7 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="77"/>
       <c r="B26" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>66</v>
@@ -2804,23 +2663,23 @@
         <v>31</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I26" s="78">
         <v>298</v>
       </c>
-      <c r="J26" s="79" t="s">
-        <v>98</v>
+      <c r="J26" s="79">
+        <v>50</v>
       </c>
       <c r="K26" s="79"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O26" s="2"/>
-      <c r="P26" s="83" t="s">
-        <v>103</v>
+      <c r="P26" s="82" t="s">
+        <v>89</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -2830,7 +2689,7 @@
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="77"/>
       <c r="B27" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>66</v>
@@ -2844,23 +2703,23 @@
         <v>31</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I27" s="78">
         <v>298</v>
       </c>
-      <c r="J27" s="79" t="s">
-        <v>98</v>
+      <c r="J27" s="79">
+        <v>50</v>
       </c>
       <c r="K27" s="79"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O27" s="2"/>
-      <c r="P27" s="83" t="s">
-        <v>100</v>
+      <c r="P27" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -2870,7 +2729,7 @@
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="77"/>
       <c r="B28" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>66</v>
@@ -2884,23 +2743,23 @@
         <v>31</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I28" s="78">
         <v>298</v>
       </c>
-      <c r="J28" s="79" t="s">
-        <v>98</v>
+      <c r="J28" s="79">
+        <v>50</v>
       </c>
       <c r="K28" s="79"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O28" s="2"/>
-      <c r="P28" s="83" t="s">
-        <v>100</v>
+      <c r="P28" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -2910,7 +2769,7 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="77"/>
       <c r="B29" s="6" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>66</v>
@@ -2927,14 +2786,14 @@
       <c r="I29" s="78">
         <v>298</v>
       </c>
-      <c r="J29" s="79" t="s">
-        <v>107</v>
+      <c r="J29" s="79">
+        <v>12</v>
       </c>
       <c r="K29" s="79"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="5">
@@ -2948,7 +2807,7 @@
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="77"/>
       <c r="B30" s="6" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>66</v>
@@ -2965,14 +2824,14 @@
       <c r="I30" s="78">
         <v>298</v>
       </c>
-      <c r="J30" s="79" t="s">
-        <v>109</v>
+      <c r="J30" s="79">
+        <v>33</v>
       </c>
       <c r="K30" s="79"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="5">
@@ -2986,7 +2845,7 @@
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="77"/>
       <c r="B31" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>66</v>
@@ -3003,14 +2862,14 @@
       <c r="I31" s="78">
         <v>298</v>
       </c>
-      <c r="J31" s="79" t="s">
-        <v>112</v>
+      <c r="J31" s="79">
+        <v>30</v>
       </c>
       <c r="K31" s="79"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="5">
@@ -3024,7 +2883,7 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="77"/>
       <c r="B32" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>66</v>
@@ -3041,14 +2900,14 @@
       <c r="I32" s="78">
         <v>298</v>
       </c>
-      <c r="J32" s="79" t="s">
-        <v>114</v>
+      <c r="J32" s="79">
+        <v>28</v>
       </c>
       <c r="K32" s="79"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="5">
@@ -3062,7 +2921,7 @@
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="77"/>
       <c r="B33" s="6" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>66</v>
@@ -3079,14 +2938,14 @@
       <c r="I33" s="78">
         <v>298</v>
       </c>
-      <c r="J33" s="79" t="s">
-        <v>84</v>
+      <c r="J33" s="79">
+        <v>29</v>
       </c>
       <c r="K33" s="79"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="5">
@@ -3100,7 +2959,7 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="77"/>
       <c r="B34" s="6" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>66</v>
@@ -3117,14 +2976,14 @@
       <c r="I34" s="78">
         <v>298</v>
       </c>
-      <c r="J34" s="79" t="s">
-        <v>117</v>
+      <c r="J34" s="79">
+        <v>26</v>
       </c>
       <c r="K34" s="79"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="5">
@@ -3138,7 +2997,7 @@
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="77"/>
       <c r="B35" s="6" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>66</v>
@@ -3155,14 +3014,14 @@
       <c r="I35" s="78">
         <v>298</v>
       </c>
-      <c r="J35" s="79" t="s">
-        <v>119</v>
+      <c r="J35" s="79">
+        <v>20</v>
       </c>
       <c r="K35" s="79"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="5">
@@ -3176,7 +3035,7 @@
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="77"/>
       <c r="B36" s="6" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>66</v>
@@ -3193,14 +3052,14 @@
       <c r="I36" s="78">
         <v>298</v>
       </c>
-      <c r="J36" s="79" t="s">
-        <v>121</v>
+      <c r="J36" s="79">
+        <v>23</v>
       </c>
       <c r="K36" s="79"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="5">
@@ -3214,7 +3073,7 @@
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="77"/>
       <c r="B37" s="6" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>66</v>
@@ -3231,14 +3090,14 @@
       <c r="I37" s="78">
         <v>298</v>
       </c>
-      <c r="J37" s="79" t="s">
-        <v>80</v>
+      <c r="J37" s="79">
+        <v>24</v>
       </c>
       <c r="K37" s="79"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="5">
@@ -3252,7 +3111,7 @@
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="77"/>
       <c r="B38" s="6" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>66</v>
@@ -3266,23 +3125,23 @@
         <v>31</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I38" s="78">
         <v>298</v>
       </c>
-      <c r="J38" s="79" t="s">
-        <v>98</v>
+      <c r="J38" s="79">
+        <v>50</v>
       </c>
       <c r="K38" s="79"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="O38" s="2"/>
-      <c r="P38" s="83" t="s">
-        <v>100</v>
+      <c r="P38" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
@@ -3292,7 +3151,7 @@
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="77"/>
       <c r="B39" s="6" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>66</v>
@@ -3309,14 +3168,14 @@
       <c r="I39" s="78">
         <v>298</v>
       </c>
-      <c r="J39" s="79" t="s">
-        <v>119</v>
+      <c r="J39" s="79">
+        <v>20</v>
       </c>
       <c r="K39" s="79"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="5">
@@ -3330,7 +3189,7 @@
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="77"/>
       <c r="B40" s="6" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>66</v>
@@ -3347,14 +3206,14 @@
       <c r="I40" s="78">
         <v>298</v>
       </c>
-      <c r="J40" s="79" t="s">
-        <v>107</v>
+      <c r="J40" s="79">
+        <v>12</v>
       </c>
       <c r="K40" s="79"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="5">
@@ -3368,7 +3227,7 @@
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="77"/>
       <c r="B41" s="6" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>66</v>
@@ -3382,23 +3241,23 @@
         <v>31</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I41" s="78">
         <v>298</v>
       </c>
-      <c r="J41" s="79" t="s">
-        <v>98</v>
+      <c r="J41" s="79">
+        <v>50</v>
       </c>
       <c r="K41" s="79"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="O41" s="2"/>
-      <c r="P41" s="83" t="s">
-        <v>100</v>
+      <c r="P41" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -3408,7 +3267,7 @@
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="77"/>
       <c r="B42" s="6" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>66</v>
@@ -3422,23 +3281,23 @@
         <v>31</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I42" s="78">
         <v>298</v>
       </c>
-      <c r="J42" s="79" t="s">
-        <v>98</v>
+      <c r="J42" s="79">
+        <v>50</v>
       </c>
       <c r="K42" s="79"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="O42" s="2"/>
-      <c r="P42" s="83" t="s">
-        <v>100</v>
+      <c r="P42" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -3448,7 +3307,7 @@
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="77"/>
       <c r="B43" s="6" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>66</v>
@@ -3465,17 +3324,17 @@
       <c r="I43" s="78">
         <v>298</v>
       </c>
-      <c r="J43" s="79" t="s">
-        <v>131</v>
+      <c r="J43" s="79">
+        <v>25.62</v>
       </c>
       <c r="K43" s="79"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="O43" s="2"/>
-      <c r="P43" s="80">
+      <c r="P43" s="7">
         <v>25.62</v>
       </c>
       <c r="Q43" s="2"/>
@@ -3486,7 +3345,7 @@
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="77"/>
       <c r="B44" s="6" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>66</v>
@@ -3503,17 +3362,17 @@
       <c r="I44" s="78">
         <v>298</v>
       </c>
-      <c r="J44" s="79" t="s">
-        <v>133</v>
+      <c r="J44" s="79">
+        <v>29.6</v>
       </c>
       <c r="K44" s="79"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="O44" s="2"/>
-      <c r="P44" s="80">
+      <c r="P44" s="7">
         <v>29.6</v>
       </c>
       <c r="Q44" s="2"/>
@@ -3524,7 +3383,7 @@
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="77"/>
       <c r="B45" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>66</v>
@@ -3541,17 +3400,17 @@
       <c r="I45" s="78">
         <v>298</v>
       </c>
-      <c r="J45" s="79" t="s">
-        <v>135</v>
+      <c r="J45" s="79">
+        <v>10.2</v>
       </c>
       <c r="K45" s="79"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="O45" s="2"/>
-      <c r="P45" s="80">
+      <c r="P45" s="7">
         <v>10.2</v>
       </c>
       <c r="Q45" s="2"/>
@@ -3562,7 +3421,7 @@
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="77"/>
       <c r="B46" s="6" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>66</v>
@@ -3579,17 +3438,17 @@
       <c r="I46" s="78">
         <v>298</v>
       </c>
-      <c r="J46" s="79" t="s">
-        <v>138</v>
+      <c r="J46" s="79">
+        <v>10.6</v>
       </c>
       <c r="K46" s="79"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="O46" s="2"/>
-      <c r="P46" s="80">
+      <c r="P46" s="7">
         <v>10.6</v>
       </c>
       <c r="Q46" s="2"/>
@@ -3600,7 +3459,7 @@
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="77"/>
       <c r="B47" s="6" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>66</v>
@@ -3617,17 +3476,17 @@
       <c r="I47" s="78">
         <v>298</v>
       </c>
-      <c r="J47" s="79" t="s">
-        <v>141</v>
+      <c r="J47" s="79">
+        <v>14.1</v>
       </c>
       <c r="K47" s="79"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="O47" s="2"/>
-      <c r="P47" s="80">
+      <c r="P47" s="7">
         <v>14.1</v>
       </c>
       <c r="Q47" s="2"/>
@@ -3655,17 +3514,17 @@
       <c r="I48" s="78">
         <v>298</v>
       </c>
-      <c r="J48" s="79" t="s">
-        <v>142</v>
+      <c r="J48" s="79">
+        <v>2.6</v>
       </c>
       <c r="K48" s="79"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="O48" s="2"/>
-      <c r="P48" s="80">
+      <c r="P48" s="7">
         <v>2.6</v>
       </c>
       <c r="Q48" s="2"/>
@@ -3676,7 +3535,7 @@
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="77"/>
       <c r="B49" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>66</v>
@@ -3693,17 +3552,17 @@
       <c r="I49" s="78">
         <v>298</v>
       </c>
-      <c r="J49" s="79" t="s">
-        <v>71</v>
+      <c r="J49" s="79">
+        <v>1.7</v>
       </c>
       <c r="K49" s="79"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="O49" s="2"/>
-      <c r="P49" s="80">
+      <c r="P49" s="7">
         <v>1.7</v>
       </c>
       <c r="Q49" s="2"/>
@@ -3714,7 +3573,7 @@
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="77"/>
       <c r="B50" s="6" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>66</v>
@@ -3728,23 +3587,23 @@
         <v>31</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I50" s="78">
         <v>298</v>
       </c>
-      <c r="J50" s="79" t="s">
-        <v>98</v>
+      <c r="J50" s="79">
+        <v>50</v>
       </c>
       <c r="K50" s="79"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O50" s="2"/>
-      <c r="P50" s="83" t="s">
-        <v>100</v>
+      <c r="P50" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
@@ -3754,7 +3613,7 @@
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="77"/>
       <c r="B51" s="6" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>66</v>
@@ -3771,14 +3630,14 @@
       <c r="I51" s="78">
         <v>298</v>
       </c>
-      <c r="J51" s="79" t="s">
-        <v>145</v>
+      <c r="J51" s="79">
+        <v>45</v>
       </c>
       <c r="K51" s="79"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="5">
@@ -3792,7 +3651,7 @@
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="77"/>
       <c r="B52" s="6" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>66</v>
@@ -3809,14 +3668,14 @@
       <c r="I52" s="78">
         <v>298</v>
       </c>
-      <c r="J52" s="79" t="s">
-        <v>147</v>
+      <c r="J52" s="79">
+        <v>42</v>
       </c>
       <c r="K52" s="79"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="5">
@@ -3830,7 +3689,7 @@
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="77"/>
       <c r="B53" s="6" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>66</v>
@@ -3847,14 +3706,14 @@
       <c r="I53" s="78">
         <v>298</v>
       </c>
-      <c r="J53" s="79" t="s">
-        <v>149</v>
+      <c r="J53" s="79">
+        <v>32</v>
       </c>
       <c r="K53" s="79"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="5">
@@ -3868,7 +3727,7 @@
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="77"/>
       <c r="B54" s="6" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>66</v>
@@ -3885,14 +3744,14 @@
       <c r="I54" s="78">
         <v>298</v>
       </c>
-      <c r="J54" s="79" t="s">
-        <v>149</v>
+      <c r="J54" s="79">
+        <v>32</v>
       </c>
       <c r="K54" s="79"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="5">
@@ -3906,7 +3765,7 @@
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="77"/>
       <c r="B55" s="6" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>66</v>
@@ -3923,14 +3782,14 @@
       <c r="I55" s="78">
         <v>298</v>
       </c>
-      <c r="J55" s="79" t="s">
-        <v>149</v>
+      <c r="J55" s="79">
+        <v>32</v>
       </c>
       <c r="K55" s="79"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="5">
@@ -3944,7 +3803,7 @@
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="77"/>
       <c r="B56" s="6" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>66</v>
@@ -3961,14 +3820,14 @@
       <c r="I56" s="78">
         <v>298</v>
       </c>
-      <c r="J56" s="79" t="s">
-        <v>112</v>
+      <c r="J56" s="79">
+        <v>30</v>
       </c>
       <c r="K56" s="79"/>
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="5">
@@ -3982,7 +3841,7 @@
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="77"/>
       <c r="B57" s="6" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>66</v>
@@ -3999,14 +3858,14 @@
       <c r="I57" s="78">
         <v>298</v>
       </c>
-      <c r="J57" s="79" t="s">
-        <v>145</v>
+      <c r="J57" s="79">
+        <v>45</v>
       </c>
       <c r="K57" s="79"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="5">
@@ -4020,7 +3879,7 @@
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="77"/>
       <c r="B58" s="6" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>66</v>
@@ -4034,23 +3893,23 @@
         <v>31</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I58" s="78">
         <v>298</v>
       </c>
-      <c r="J58" s="79" t="s">
-        <v>98</v>
+      <c r="J58" s="79">
+        <v>50</v>
       </c>
       <c r="K58" s="79"/>
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="N58" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O58" s="2"/>
-      <c r="P58" s="83" t="s">
-        <v>100</v>
+      <c r="P58" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -4060,7 +3919,7 @@
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="77"/>
       <c r="B59" s="6" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>66</v>
@@ -4077,14 +3936,14 @@
       <c r="I59" s="78">
         <v>298</v>
       </c>
-      <c r="J59" s="79" t="s">
-        <v>155</v>
+      <c r="J59" s="79">
+        <v>43</v>
       </c>
       <c r="K59" s="79"/>
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="5">
@@ -4098,7 +3957,7 @@
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="77"/>
       <c r="B60" s="6" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>66</v>
@@ -4115,17 +3974,17 @@
       <c r="I60" s="78">
         <v>298</v>
       </c>
-      <c r="J60" s="79" t="s">
-        <v>157</v>
+      <c r="J60" s="79">
+        <v>26.6</v>
       </c>
       <c r="K60" s="79"/>
       <c r="L60" s="6"/>
       <c r="M60" s="6"/>
       <c r="N60" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O60" s="2"/>
-      <c r="P60" s="80">
+      <c r="P60" s="7">
         <v>26.6</v>
       </c>
       <c r="Q60" s="2"/>
@@ -4136,7 +3995,7 @@
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="77"/>
       <c r="B61" s="6" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>66</v>
@@ -4153,14 +4012,14 @@
       <c r="I61" s="78">
         <v>298</v>
       </c>
-      <c r="J61" s="79" t="s">
-        <v>159</v>
+      <c r="J61" s="79">
+        <v>25</v>
       </c>
       <c r="K61" s="79"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
       <c r="N61" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="5">
@@ -4174,7 +4033,7 @@
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="77"/>
       <c r="B62" s="6" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>66</v>
@@ -4191,14 +4050,14 @@
       <c r="I62" s="78">
         <v>298</v>
       </c>
-      <c r="J62" s="79" t="s">
-        <v>119</v>
+      <c r="J62" s="79">
+        <v>20</v>
       </c>
       <c r="K62" s="79"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="5">
@@ -4212,7 +4071,7 @@
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="77"/>
       <c r="B63" s="6" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>66</v>
@@ -4229,14 +4088,14 @@
       <c r="I63" s="78">
         <v>298</v>
       </c>
-      <c r="J63" s="79" t="s">
-        <v>162</v>
+      <c r="J63" s="79">
+        <v>8</v>
       </c>
       <c r="K63" s="79"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="5">
@@ -4250,7 +4109,7 @@
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="77"/>
       <c r="B64" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>66</v>
@@ -4267,17 +4126,17 @@
       <c r="I64" s="78">
         <v>298</v>
       </c>
-      <c r="J64" s="79" t="s">
-        <v>93</v>
+      <c r="J64" s="79">
+        <v>24.61</v>
       </c>
       <c r="K64" s="79"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
       <c r="N64" s="6" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="O64" s="2"/>
-      <c r="P64" s="80">
+      <c r="P64" s="7">
         <v>24.61</v>
       </c>
       <c r="Q64" s="2"/>
@@ -4288,7 +4147,7 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="77"/>
       <c r="B65" s="6" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>66</v>
@@ -4305,14 +4164,14 @@
       <c r="I65" s="78">
         <v>298</v>
       </c>
-      <c r="J65" s="79" t="s">
-        <v>165</v>
+      <c r="J65" s="79">
+        <v>34</v>
       </c>
       <c r="K65" s="79"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" s="5">
@@ -4343,17 +4202,17 @@
       <c r="I66" s="78">
         <v>298</v>
       </c>
-      <c r="J66" s="79" t="s">
-        <v>167</v>
+      <c r="J66" s="79">
+        <v>1.9</v>
       </c>
       <c r="K66" s="79"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="O66" s="2"/>
-      <c r="P66" s="80">
+      <c r="P66" s="7">
         <v>1.9</v>
       </c>
       <c r="Q66" s="2"/>
@@ -4364,7 +4223,7 @@
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="77"/>
       <c r="B67" s="6" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>66</v>
@@ -4381,17 +4240,17 @@
       <c r="I67" s="78">
         <v>298</v>
       </c>
-      <c r="J67" s="79" t="s">
-        <v>170</v>
+      <c r="J67" s="79">
+        <v>2.5</v>
       </c>
       <c r="K67" s="79"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
       <c r="N67" s="6" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="O67" s="2"/>
-      <c r="P67" s="80">
+      <c r="P67" s="7">
         <v>2.5</v>
       </c>
       <c r="Q67" s="2"/>
@@ -4402,7 +4261,7 @@
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="77"/>
       <c r="B68" s="6" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>66</v>
@@ -4419,17 +4278,17 @@
       <c r="I68" s="78">
         <v>298</v>
       </c>
-      <c r="J68" s="79" t="s">
-        <v>172</v>
+      <c r="J68" s="79">
+        <v>5.9</v>
       </c>
       <c r="K68" s="79"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="O68" s="2"/>
-      <c r="P68" s="80">
+      <c r="P68" s="7">
         <v>5.9</v>
       </c>
       <c r="Q68" s="2"/>
@@ -4440,7 +4299,7 @@
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="77"/>
       <c r="B69" s="6" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>66</v>
@@ -4457,17 +4316,17 @@
       <c r="I69" s="78">
         <v>298</v>
       </c>
-      <c r="J69" s="79" t="s">
-        <v>174</v>
+      <c r="J69" s="79">
+        <v>8.4</v>
       </c>
       <c r="K69" s="79"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="O69" s="2"/>
-      <c r="P69" s="80">
+      <c r="P69" s="7">
         <v>8.4</v>
       </c>
       <c r="Q69" s="2"/>
@@ -4478,7 +4337,7 @@
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="77"/>
       <c r="B70" s="6" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>66</v>
@@ -4495,17 +4354,17 @@
       <c r="I70" s="78">
         <v>298</v>
       </c>
-      <c r="J70" s="79" t="s">
-        <v>175</v>
+      <c r="J70" s="79">
+        <v>11.5</v>
       </c>
       <c r="K70" s="79"/>
       <c r="L70" s="6"/>
       <c r="M70" s="6"/>
       <c r="N70" s="6" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="O70" s="2"/>
-      <c r="P70" s="80">
+      <c r="P70" s="7">
         <v>11.5</v>
       </c>
       <c r="Q70" s="2"/>
@@ -4516,7 +4375,7 @@
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="77"/>
       <c r="B71" s="6" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>66</v>
@@ -4533,14 +4392,14 @@
       <c r="I71" s="78">
         <v>298</v>
       </c>
-      <c r="J71" s="79" t="s">
-        <v>112</v>
+      <c r="J71" s="79">
+        <v>30</v>
       </c>
       <c r="K71" s="79"/>
       <c r="L71" s="6"/>
       <c r="M71" s="6"/>
       <c r="N71" s="6" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" s="5">
@@ -4554,7 +4413,7 @@
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="77"/>
       <c r="B72" s="6" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>66</v>
@@ -4562,7 +4421,7 @@
       <c r="D72" s="3"/>
       <c r="E72" s="5"/>
       <c r="F72" s="3" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>31</v>
@@ -4571,17 +4430,17 @@
       <c r="I72" s="78">
         <v>298</v>
       </c>
-      <c r="J72" s="79" t="s">
-        <v>180</v>
+      <c r="J72" s="79">
+        <v>20.6</v>
       </c>
       <c r="K72" s="79"/>
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
       <c r="N72" s="6" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="O72" s="2"/>
-      <c r="P72" s="80">
+      <c r="P72" s="7">
         <v>20.6</v>
       </c>
       <c r="Q72" s="2"/>
@@ -4592,7 +4451,7 @@
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="77"/>
       <c r="B73" s="6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>66</v>
@@ -4600,7 +4459,7 @@
       <c r="D73" s="3"/>
       <c r="E73" s="5"/>
       <c r="F73" s="3" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>31</v>
@@ -4609,17 +4468,17 @@
       <c r="I73" s="78">
         <v>298</v>
       </c>
-      <c r="J73" s="79" t="s">
-        <v>182</v>
+      <c r="J73" s="79">
+        <v>9.7</v>
       </c>
       <c r="K73" s="79"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
       <c r="N73" s="6" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="O73" s="2"/>
-      <c r="P73" s="80">
+      <c r="P73" s="7">
         <v>9.7</v>
       </c>
       <c r="Q73" s="2"/>
@@ -4630,7 +4489,7 @@
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="77"/>
       <c r="B74" s="6" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>66</v>
@@ -4638,7 +4497,7 @@
       <c r="D74" s="3"/>
       <c r="E74" s="5"/>
       <c r="F74" s="3" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>31</v>
@@ -4647,17 +4506,17 @@
       <c r="I74" s="78">
         <v>298</v>
       </c>
-      <c r="J74" s="79" t="s">
-        <v>185</v>
+      <c r="J74" s="79">
+        <v>14.9</v>
       </c>
       <c r="K74" s="79"/>
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
       <c r="N74" s="6" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="O74" s="2"/>
-      <c r="P74" s="80">
+      <c r="P74" s="7">
         <v>14.9</v>
       </c>
       <c r="Q74" s="2"/>
@@ -4668,7 +4527,7 @@
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="77"/>
       <c r="B75" s="6" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>66</v>
@@ -4676,7 +4535,7 @@
       <c r="D75" s="3"/>
       <c r="E75" s="5"/>
       <c r="F75" s="3" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>31</v>
@@ -4685,17 +4544,17 @@
       <c r="I75" s="78">
         <v>298</v>
       </c>
-      <c r="J75" s="79" t="s">
-        <v>188</v>
+      <c r="J75" s="79">
+        <v>18.8</v>
       </c>
       <c r="K75" s="79"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
       <c r="N75" s="6" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="O75" s="2"/>
-      <c r="P75" s="80">
+      <c r="P75" s="7">
         <v>18.8</v>
       </c>
       <c r="Q75" s="2"/>

</xml_diff>